<commit_message>
Added work to convert sklearn model to pyspark machine learning
</commit_message>
<xml_diff>
--- a/612 report work distribution.xlsx
+++ b/612 report work distribution.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hatter\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Masters Stuff\ENSF612\team project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Section</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Adding a heuristic feature and run model</t>
+  </si>
+  <si>
+    <t>Convert model from sklearn to pyspark</t>
   </si>
 </sst>
 </file>
@@ -404,17 +407,17 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="84.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -442,7 +445,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -453,7 +456,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -464,15 +467,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -480,7 +486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -488,7 +494,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -496,7 +502,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -504,7 +510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Took on grid search and parameter tuning
</commit_message>
<xml_diff>
--- a/612 report work distribution.xlsx
+++ b/612 report work distribution.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Masters Stuff\ENSF612\team project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lancelot\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5430"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Section</t>
   </si>
@@ -406,18 +406,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -445,7 +445,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -455,8 +455,11 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -467,7 +470,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -478,7 +481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -486,7 +489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -494,7 +497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -502,7 +505,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -510,7 +513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>

</xml_diff>